<commit_message>
05/05 - push code
Signed-off-by: Nguyễn Minh Hiếu <hieu000502@gmail.com>
</commit_message>
<xml_diff>
--- a/wfms/src/main/resources/templates/template_users.xlsx
+++ b/wfms/src/main/resources/templates/template_users.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\DuAnHocThem\DoAnQuanLyCongViec\swp490_g5_be\wfms\src\main\resources\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf59153fc7b6c1fa/Máy tính/wfms/swp490_g5_be/wfms/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FA574C-9350-4721-937C-B0EC1BF11C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="13_ncr:1_{B2FA574C-9350-4721-937C-B0EC1BF11C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BE18015-C9B3-4845-82FA-697B2E46C687}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D34DD7CE-52D2-46B1-B543-9BB9ED1B736D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{D34DD7CE-52D2-46B1-B543-9BB9ED1B736D}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -33,36 +33,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t xml:space="preserve">Tên nhân viên </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Địa chỉ </t>
-  </si>
-  <si>
-    <t>Giới tính</t>
-  </si>
-  <si>
-    <t>Địa chỉ email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Số điện thoại </t>
-  </si>
-  <si>
-    <t>Ngày sinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Công việc </t>
-  </si>
-  <si>
-    <t>userId</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>username</t>
   </si>
@@ -85,10 +72,34 @@
     <t>jobTitle</t>
   </si>
   <si>
-    <t xml:space="preserve">Nhân viên </t>
+    <t>fullName</t>
   </si>
   <si>
-    <t>user</t>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone number</t>
+  </si>
+  <si>
+    <t>Day of birth</t>
+  </si>
+  <si>
+    <t>Job title</t>
+  </si>
+  <si>
+    <t>Full name</t>
   </si>
 </sst>
 </file>
@@ -418,6 +429,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -717,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D885B9B-C28B-4173-85C4-C911572856AF}">
-  <dimension ref="A1:H100"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -732,35 +747,39 @@
     <col min="5" max="6" width="18.88671875" customWidth="1"/>
     <col min="7" max="7" width="16.88671875" customWidth="1"/>
     <col min="8" max="8" width="21.109375" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" t="str">
         <f>IF(A2="","",VLOOKUP(A2,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -789,8 +808,12 @@
         <f>IF(A2="","",VLOOKUP(A2,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" t="str">
+        <f>IF(A2="","",VLOOKUP(A2,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="str">
         <f>IF(A3="","",VLOOKUP(A3,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -819,8 +842,12 @@
         <f>IF(A3="","",VLOOKUP(A3,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" t="str">
+        <f>IF(A3="","",VLOOKUP(A3,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" t="str">
         <f>IF(A4="","",VLOOKUP(A4,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -849,8 +876,12 @@
         <f>IF(A4="","",VLOOKUP(A4,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" t="str">
+        <f>IF(A4="","",VLOOKUP(A4,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" t="str">
         <f>IF(A5="","",VLOOKUP(A5,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -879,8 +910,12 @@
         <f>IF(A5="","",VLOOKUP(A5,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" t="str">
+        <f>IF(A5="","",VLOOKUP(A5,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" t="str">
         <f>IF(A6="","",VLOOKUP(A6,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -909,8 +944,12 @@
         <f>IF(A6="","",VLOOKUP(A6,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" t="str">
+        <f>IF(A6="","",VLOOKUP(A6,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" t="str">
         <f>IF(A7="","",VLOOKUP(A7,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -939,8 +978,12 @@
         <f>IF(A7="","",VLOOKUP(A7,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" t="str">
+        <f>IF(A7="","",VLOOKUP(A7,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" t="str">
         <f>IF(A8="","",VLOOKUP(A8,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -969,8 +1012,12 @@
         <f>IF(A8="","",VLOOKUP(A8,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" t="str">
+        <f>IF(A8="","",VLOOKUP(A8,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" t="str">
         <f>IF(A9="","",VLOOKUP(A9,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -999,8 +1046,12 @@
         <f>IF(A9="","",VLOOKUP(A9,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" t="str">
+        <f>IF(A9="","",VLOOKUP(A9,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" t="str">
         <f>IF(A10="","",VLOOKUP(A10,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1029,8 +1080,12 @@
         <f>IF(A10="","",VLOOKUP(A10,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" t="str">
+        <f>IF(A10="","",VLOOKUP(A10,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" t="str">
         <f>IF(A11="","",VLOOKUP(A11,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1059,8 +1114,12 @@
         <f>IF(A11="","",VLOOKUP(A11,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11" t="str">
+        <f>IF(A11="","",VLOOKUP(A11,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
         <f>IF(A12="","",VLOOKUP(A12,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1089,8 +1148,12 @@
         <f>IF(A12="","",VLOOKUP(A12,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" t="str">
+        <f>IF(A12="","",VLOOKUP(A12,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <f>IF(A13="","",VLOOKUP(A13,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1119,8 +1182,12 @@
         <f>IF(A13="","",VLOOKUP(A13,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13" t="str">
+        <f>IF(A13="","",VLOOKUP(A13,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" t="str">
         <f>IF(A14="","",VLOOKUP(A14,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1149,8 +1216,12 @@
         <f>IF(A14="","",VLOOKUP(A14,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14" t="str">
+        <f>IF(A14="","",VLOOKUP(A14,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" t="str">
         <f>IF(A15="","",VLOOKUP(A15,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1179,8 +1250,12 @@
         <f>IF(A15="","",VLOOKUP(A15,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15" t="str">
+        <f>IF(A15="","",VLOOKUP(A15,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" t="str">
         <f>IF(A16="","",VLOOKUP(A16,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1209,8 +1284,12 @@
         <f>IF(A16="","",VLOOKUP(A16,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I16" t="str">
+        <f>IF(A16="","",VLOOKUP(A16,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" t="str">
         <f>IF(A17="","",VLOOKUP(A17,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1239,8 +1318,12 @@
         <f>IF(A17="","",VLOOKUP(A17,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I17" t="str">
+        <f>IF(A17="","",VLOOKUP(A17,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
         <f>IF(A18="","",VLOOKUP(A18,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1269,8 +1352,12 @@
         <f>IF(A18="","",VLOOKUP(A18,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I18" t="str">
+        <f>IF(A18="","",VLOOKUP(A18,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
         <f>IF(A19="","",VLOOKUP(A19,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1299,8 +1386,12 @@
         <f>IF(A19="","",VLOOKUP(A19,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I19" t="str">
+        <f>IF(A19="","",VLOOKUP(A19,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
         <f>IF(A20="","",VLOOKUP(A20,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1329,8 +1420,12 @@
         <f>IF(A20="","",VLOOKUP(A20,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I20" t="str">
+        <f>IF(A20="","",VLOOKUP(A20,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
         <f>IF(A21="","",VLOOKUP(A21,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1359,8 +1454,12 @@
         <f>IF(A21="","",VLOOKUP(A21,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I21" t="str">
+        <f>IF(A21="","",VLOOKUP(A21,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
         <f>IF(A22="","",VLOOKUP(A22,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1389,8 +1488,12 @@
         <f>IF(A22="","",VLOOKUP(A22,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I22" t="str">
+        <f>IF(A22="","",VLOOKUP(A22,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
         <f>IF(A23="","",VLOOKUP(A23,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1419,8 +1522,12 @@
         <f>IF(A23="","",VLOOKUP(A23,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I23" t="str">
+        <f>IF(A23="","",VLOOKUP(A23,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
         <f>IF(A24="","",VLOOKUP(A24,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1449,8 +1556,12 @@
         <f>IF(A24="","",VLOOKUP(A24,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I24" t="str">
+        <f>IF(A24="","",VLOOKUP(A24,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
         <f>IF(A25="","",VLOOKUP(A25,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1479,8 +1590,12 @@
         <f>IF(A25="","",VLOOKUP(A25,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I25" t="str">
+        <f>IF(A25="","",VLOOKUP(A25,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
         <f>IF(A26="","",VLOOKUP(A26,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1509,8 +1624,12 @@
         <f>IF(A26="","",VLOOKUP(A26,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I26" t="str">
+        <f>IF(A26="","",VLOOKUP(A26,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
         <f>IF(A27="","",VLOOKUP(A27,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1539,8 +1658,12 @@
         <f>IF(A27="","",VLOOKUP(A27,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I27" t="str">
+        <f>IF(A27="","",VLOOKUP(A27,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
         <f>IF(A28="","",VLOOKUP(A28,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1569,8 +1692,12 @@
         <f>IF(A28="","",VLOOKUP(A28,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I28" t="str">
+        <f>IF(A28="","",VLOOKUP(A28,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" t="str">
         <f>IF(A29="","",VLOOKUP(A29,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1599,8 +1726,12 @@
         <f>IF(A29="","",VLOOKUP(A29,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I29" t="str">
+        <f>IF(A29="","",VLOOKUP(A29,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" t="str">
         <f>IF(A30="","",VLOOKUP(A30,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1629,8 +1760,12 @@
         <f>IF(A30="","",VLOOKUP(A30,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I30" t="str">
+        <f>IF(A30="","",VLOOKUP(A30,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
         <f>IF(A31="","",VLOOKUP(A31,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1659,8 +1794,12 @@
         <f>IF(A31="","",VLOOKUP(A31,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I31" t="str">
+        <f>IF(A31="","",VLOOKUP(A31,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <f>IF(A32="","",VLOOKUP(A32,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1689,8 +1828,12 @@
         <f>IF(A32="","",VLOOKUP(A32,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I32" t="str">
+        <f>IF(A32="","",VLOOKUP(A32,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
         <f>IF(A33="","",VLOOKUP(A33,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1719,8 +1862,12 @@
         <f>IF(A33="","",VLOOKUP(A33,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I33" t="str">
+        <f>IF(A33="","",VLOOKUP(A33,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
         <f>IF(A34="","",VLOOKUP(A34,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1749,8 +1896,12 @@
         <f>IF(A34="","",VLOOKUP(A34,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I34" t="str">
+        <f>IF(A34="","",VLOOKUP(A34,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
         <f>IF(A35="","",VLOOKUP(A35,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1779,8 +1930,12 @@
         <f>IF(A35="","",VLOOKUP(A35,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I35" t="str">
+        <f>IF(A35="","",VLOOKUP(A35,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B36" t="str">
         <f>IF(A36="","",VLOOKUP(A36,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1809,8 +1964,12 @@
         <f>IF(A36="","",VLOOKUP(A36,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I36" t="str">
+        <f>IF(A36="","",VLOOKUP(A36,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B37" t="str">
         <f>IF(A37="","",VLOOKUP(A37,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1839,8 +1998,12 @@
         <f>IF(A37="","",VLOOKUP(A37,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I37" t="str">
+        <f>IF(A37="","",VLOOKUP(A37,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B38" t="str">
         <f>IF(A38="","",VLOOKUP(A38,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1869,8 +2032,12 @@
         <f>IF(A38="","",VLOOKUP(A38,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I38" t="str">
+        <f>IF(A38="","",VLOOKUP(A38,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B39" t="str">
         <f>IF(A39="","",VLOOKUP(A39,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1899,8 +2066,12 @@
         <f>IF(A39="","",VLOOKUP(A39,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I39" t="str">
+        <f>IF(A39="","",VLOOKUP(A39,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B40" t="str">
         <f>IF(A40="","",VLOOKUP(A40,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1929,8 +2100,12 @@
         <f>IF(A40="","",VLOOKUP(A40,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I40" t="str">
+        <f>IF(A40="","",VLOOKUP(A40,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B41" t="str">
         <f>IF(A41="","",VLOOKUP(A41,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1959,8 +2134,12 @@
         <f>IF(A41="","",VLOOKUP(A41,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I41" t="str">
+        <f>IF(A41="","",VLOOKUP(A41,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B42" t="str">
         <f>IF(A42="","",VLOOKUP(A42,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -1989,8 +2168,12 @@
         <f>IF(A42="","",VLOOKUP(A42,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I42" t="str">
+        <f>IF(A42="","",VLOOKUP(A42,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B43" t="str">
         <f>IF(A43="","",VLOOKUP(A43,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2019,8 +2202,12 @@
         <f>IF(A43="","",VLOOKUP(A43,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I43" t="str">
+        <f>IF(A43="","",VLOOKUP(A43,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44" t="str">
         <f>IF(A44="","",VLOOKUP(A44,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2049,8 +2236,12 @@
         <f>IF(A44="","",VLOOKUP(A44,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I44" t="str">
+        <f>IF(A44="","",VLOOKUP(A44,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B45" t="str">
         <f>IF(A45="","",VLOOKUP(A45,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2079,8 +2270,12 @@
         <f>IF(A45="","",VLOOKUP(A45,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I45" t="str">
+        <f>IF(A45="","",VLOOKUP(A45,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B46" t="str">
         <f>IF(A46="","",VLOOKUP(A46,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2109,8 +2304,12 @@
         <f>IF(A46="","",VLOOKUP(A46,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I46" t="str">
+        <f>IF(A46="","",VLOOKUP(A46,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B47" t="str">
         <f>IF(A47="","",VLOOKUP(A47,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2139,8 +2338,12 @@
         <f>IF(A47="","",VLOOKUP(A47,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I47" t="str">
+        <f>IF(A47="","",VLOOKUP(A47,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B48" t="str">
         <f>IF(A48="","",VLOOKUP(A48,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2169,8 +2372,12 @@
         <f>IF(A48="","",VLOOKUP(A48,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I48" t="str">
+        <f>IF(A48="","",VLOOKUP(A48,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B49" t="str">
         <f>IF(A49="","",VLOOKUP(A49,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2199,8 +2406,12 @@
         <f>IF(A49="","",VLOOKUP(A49,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I49" t="str">
+        <f>IF(A49="","",VLOOKUP(A49,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B50" t="str">
         <f>IF(A50="","",VLOOKUP(A50,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2229,8 +2440,12 @@
         <f>IF(A50="","",VLOOKUP(A50,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I50" t="str">
+        <f>IF(A50="","",VLOOKUP(A50,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B51" t="str">
         <f>IF(A51="","",VLOOKUP(A51,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2259,8 +2474,12 @@
         <f>IF(A51="","",VLOOKUP(A51,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I51" t="str">
+        <f>IF(A51="","",VLOOKUP(A51,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B52" t="str">
         <f>IF(A52="","",VLOOKUP(A52,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2289,8 +2508,12 @@
         <f>IF(A52="","",VLOOKUP(A52,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I52" t="str">
+        <f>IF(A52="","",VLOOKUP(A52,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B53" t="str">
         <f>IF(A53="","",VLOOKUP(A53,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2319,8 +2542,12 @@
         <f>IF(A53="","",VLOOKUP(A53,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I53" t="str">
+        <f>IF(A53="","",VLOOKUP(A53,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B54" t="str">
         <f>IF(A54="","",VLOOKUP(A54,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2349,8 +2576,12 @@
         <f>IF(A54="","",VLOOKUP(A54,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I54" t="str">
+        <f>IF(A54="","",VLOOKUP(A54,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B55" t="str">
         <f>IF(A55="","",VLOOKUP(A55,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2379,8 +2610,12 @@
         <f>IF(A55="","",VLOOKUP(A55,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I55" t="str">
+        <f>IF(A55="","",VLOOKUP(A55,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B56" t="str">
         <f>IF(A56="","",VLOOKUP(A56,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2409,8 +2644,12 @@
         <f>IF(A56="","",VLOOKUP(A56,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I56" t="str">
+        <f>IF(A56="","",VLOOKUP(A56,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B57" t="str">
         <f>IF(A57="","",VLOOKUP(A57,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2439,8 +2678,12 @@
         <f>IF(A57="","",VLOOKUP(A57,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I57" t="str">
+        <f>IF(A57="","",VLOOKUP(A57,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B58" t="str">
         <f>IF(A58="","",VLOOKUP(A58,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2469,8 +2712,12 @@
         <f>IF(A58="","",VLOOKUP(A58,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I58" t="str">
+        <f>IF(A58="","",VLOOKUP(A58,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B59" t="str">
         <f>IF(A59="","",VLOOKUP(A59,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2499,8 +2746,12 @@
         <f>IF(A59="","",VLOOKUP(A59,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I59" t="str">
+        <f>IF(A59="","",VLOOKUP(A59,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B60" t="str">
         <f>IF(A60="","",VLOOKUP(A60,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2529,8 +2780,12 @@
         <f>IF(A60="","",VLOOKUP(A60,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I60" t="str">
+        <f>IF(A60="","",VLOOKUP(A60,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B61" t="str">
         <f>IF(A61="","",VLOOKUP(A61,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2559,8 +2814,12 @@
         <f>IF(A61="","",VLOOKUP(A61,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I61" t="str">
+        <f>IF(A61="","",VLOOKUP(A61,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B62" t="str">
         <f>IF(A62="","",VLOOKUP(A62,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2589,8 +2848,12 @@
         <f>IF(A62="","",VLOOKUP(A62,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I62" t="str">
+        <f>IF(A62="","",VLOOKUP(A62,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B63" t="str">
         <f>IF(A63="","",VLOOKUP(A63,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2619,8 +2882,12 @@
         <f>IF(A63="","",VLOOKUP(A63,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I63" t="str">
+        <f>IF(A63="","",VLOOKUP(A63,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B64" t="str">
         <f>IF(A64="","",VLOOKUP(A64,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2649,8 +2916,12 @@
         <f>IF(A64="","",VLOOKUP(A64,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I64" t="str">
+        <f>IF(A64="","",VLOOKUP(A64,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B65" t="str">
         <f>IF(A65="","",VLOOKUP(A65,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2679,8 +2950,12 @@
         <f>IF(A65="","",VLOOKUP(A65,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I65" t="str">
+        <f>IF(A65="","",VLOOKUP(A65,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B66" t="str">
         <f>IF(A66="","",VLOOKUP(A66,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2709,8 +2984,12 @@
         <f>IF(A66="","",VLOOKUP(A66,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I66" t="str">
+        <f>IF(A66="","",VLOOKUP(A66,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B67" t="str">
         <f>IF(A67="","",VLOOKUP(A67,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2739,8 +3018,12 @@
         <f>IF(A67="","",VLOOKUP(A67,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I67" t="str">
+        <f>IF(A67="","",VLOOKUP(A67,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B68" t="str">
         <f>IF(A68="","",VLOOKUP(A68,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2769,8 +3052,12 @@
         <f>IF(A68="","",VLOOKUP(A68,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I68" t="str">
+        <f>IF(A68="","",VLOOKUP(A68,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B69" t="str">
         <f>IF(A69="","",VLOOKUP(A69,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2799,8 +3086,12 @@
         <f>IF(A69="","",VLOOKUP(A69,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I69" t="str">
+        <f>IF(A69="","",VLOOKUP(A69,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B70" t="str">
         <f>IF(A70="","",VLOOKUP(A70,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2829,8 +3120,12 @@
         <f>IF(A70="","",VLOOKUP(A70,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I70" t="str">
+        <f>IF(A70="","",VLOOKUP(A70,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B71" t="str">
         <f>IF(A71="","",VLOOKUP(A71,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2859,8 +3154,12 @@
         <f>IF(A71="","",VLOOKUP(A71,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I71" t="str">
+        <f>IF(A71="","",VLOOKUP(A71,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B72" t="str">
         <f>IF(A72="","",VLOOKUP(A72,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2889,8 +3188,12 @@
         <f>IF(A72="","",VLOOKUP(A72,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I72" t="str">
+        <f>IF(A72="","",VLOOKUP(A72,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B73" t="str">
         <f>IF(A73="","",VLOOKUP(A73,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2919,8 +3222,12 @@
         <f>IF(A73="","",VLOOKUP(A73,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I73" t="str">
+        <f>IF(A73="","",VLOOKUP(A73,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B74" t="str">
         <f>IF(A74="","",VLOOKUP(A74,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2949,8 +3256,12 @@
         <f>IF(A74="","",VLOOKUP(A74,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I74" t="str">
+        <f>IF(A74="","",VLOOKUP(A74,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B75" t="str">
         <f>IF(A75="","",VLOOKUP(A75,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -2979,8 +3290,12 @@
         <f>IF(A75="","",VLOOKUP(A75,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I75" t="str">
+        <f>IF(A75="","",VLOOKUP(A75,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B76" t="str">
         <f>IF(A76="","",VLOOKUP(A76,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3009,8 +3324,12 @@
         <f>IF(A76="","",VLOOKUP(A76,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I76" t="str">
+        <f>IF(A76="","",VLOOKUP(A76,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B77" t="str">
         <f>IF(A77="","",VLOOKUP(A77,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3039,8 +3358,12 @@
         <f>IF(A77="","",VLOOKUP(A77,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I77" t="str">
+        <f>IF(A77="","",VLOOKUP(A77,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B78" t="str">
         <f>IF(A78="","",VLOOKUP(A78,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3069,8 +3392,12 @@
         <f>IF(A78="","",VLOOKUP(A78,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I78" t="str">
+        <f>IF(A78="","",VLOOKUP(A78,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B79" t="str">
         <f>IF(A79="","",VLOOKUP(A79,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3099,8 +3426,12 @@
         <f>IF(A79="","",VLOOKUP(A79,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I79" t="str">
+        <f>IF(A79="","",VLOOKUP(A79,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B80" t="str">
         <f>IF(A80="","",VLOOKUP(A80,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3129,8 +3460,12 @@
         <f>IF(A80="","",VLOOKUP(A80,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I80" t="str">
+        <f>IF(A80="","",VLOOKUP(A80,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B81" t="str">
         <f>IF(A81="","",VLOOKUP(A81,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3159,8 +3494,12 @@
         <f>IF(A81="","",VLOOKUP(A81,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I81" t="str">
+        <f>IF(A81="","",VLOOKUP(A81,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B82" t="str">
         <f>IF(A82="","",VLOOKUP(A82,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3189,8 +3528,12 @@
         <f>IF(A82="","",VLOOKUP(A82,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I82" t="str">
+        <f>IF(A82="","",VLOOKUP(A82,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B83" t="str">
         <f>IF(A83="","",VLOOKUP(A83,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3219,8 +3562,12 @@
         <f>IF(A83="","",VLOOKUP(A83,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I83" t="str">
+        <f>IF(A83="","",VLOOKUP(A83,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B84" t="str">
         <f>IF(A84="","",VLOOKUP(A84,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3249,8 +3596,12 @@
         <f>IF(A84="","",VLOOKUP(A84,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I84" t="str">
+        <f>IF(A84="","",VLOOKUP(A84,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B85" t="str">
         <f>IF(A85="","",VLOOKUP(A85,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3279,8 +3630,12 @@
         <f>IF(A85="","",VLOOKUP(A85,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I85" t="str">
+        <f>IF(A85="","",VLOOKUP(A85,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B86" t="str">
         <f>IF(A86="","",VLOOKUP(A86,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3309,8 +3664,12 @@
         <f>IF(A86="","",VLOOKUP(A86,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I86" t="str">
+        <f>IF(A86="","",VLOOKUP(A86,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B87" t="str">
         <f>IF(A87="","",VLOOKUP(A87,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3339,8 +3698,12 @@
         <f>IF(A87="","",VLOOKUP(A87,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I87" t="str">
+        <f>IF(A87="","",VLOOKUP(A87,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B88" t="str">
         <f>IF(A88="","",VLOOKUP(A88,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3369,8 +3732,12 @@
         <f>IF(A88="","",VLOOKUP(A88,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I88" t="str">
+        <f>IF(A88="","",VLOOKUP(A88,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B89" t="str">
         <f>IF(A89="","",VLOOKUP(A89,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3399,8 +3766,12 @@
         <f>IF(A89="","",VLOOKUP(A89,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I89" t="str">
+        <f>IF(A89="","",VLOOKUP(A89,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B90" t="str">
         <f>IF(A90="","",VLOOKUP(A90,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3429,8 +3800,12 @@
         <f>IF(A90="","",VLOOKUP(A90,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I90" t="str">
+        <f>IF(A90="","",VLOOKUP(A90,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B91" t="str">
         <f>IF(A91="","",VLOOKUP(A91,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3459,8 +3834,12 @@
         <f>IF(A91="","",VLOOKUP(A91,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I91" t="str">
+        <f>IF(A91="","",VLOOKUP(A91,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B92" t="str">
         <f>IF(A92="","",VLOOKUP(A92,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3489,8 +3868,12 @@
         <f>IF(A92="","",VLOOKUP(A92,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I92" t="str">
+        <f>IF(A92="","",VLOOKUP(A92,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B93" t="str">
         <f>IF(A93="","",VLOOKUP(A93,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3519,8 +3902,12 @@
         <f>IF(A93="","",VLOOKUP(A93,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I93" t="str">
+        <f>IF(A93="","",VLOOKUP(A93,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B94" t="str">
         <f>IF(A94="","",VLOOKUP(A94,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3549,8 +3936,12 @@
         <f>IF(A94="","",VLOOKUP(A94,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I94" t="str">
+        <f>IF(A94="","",VLOOKUP(A94,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B95" t="str">
         <f>IF(A95="","",VLOOKUP(A95,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3579,8 +3970,12 @@
         <f>IF(A95="","",VLOOKUP(A95,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I95" t="str">
+        <f>IF(A95="","",VLOOKUP(A95,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B96" t="str">
         <f>IF(A96="","",VLOOKUP(A96,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3609,8 +4004,12 @@
         <f>IF(A96="","",VLOOKUP(A96,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I96" t="str">
+        <f>IF(A96="","",VLOOKUP(A96,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B97" t="str">
         <f>IF(A97="","",VLOOKUP(A97,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3639,8 +4038,12 @@
         <f>IF(A97="","",VLOOKUP(A97,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I97" t="str">
+        <f>IF(A97="","",VLOOKUP(A97,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B98" t="str">
         <f>IF(A98="","",VLOOKUP(A98,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3669,8 +4072,12 @@
         <f>IF(A98="","",VLOOKUP(A98,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I98" t="str">
+        <f>IF(A98="","",VLOOKUP(A98,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B99" t="str">
         <f>IF(A99="","",VLOOKUP(A99,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3699,8 +4106,12 @@
         <f>IF(A99="","",VLOOKUP(A99,Note!$A$1:$H$816,8,0))</f>
         <v/>
       </c>
-    </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I99" t="str">
+        <f>IF(A99="","",VLOOKUP(A99,Note!$A$1:$I$816,9,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B100" t="str">
         <f>IF(A100="","",VLOOKUP(A100,Note!$A$1:$H$816,2,0))</f>
         <v/>
@@ -3727,6 +4138,10 @@
       </c>
       <c r="H100" t="str">
         <f>IF(A100="","",VLOOKUP(A100,Note!$A$1:$H$816,8,0))</f>
+        <v/>
+      </c>
+      <c r="I100" t="str">
+        <f>IF(A100="","",VLOOKUP(A100,Note!$A$1:$I$816,9,0))</f>
         <v/>
       </c>
     </row>
@@ -3739,8 +4154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52667CD6-EE1F-4444-9550-699EBACD05D2}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3756,28 +4171,28 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>7</v>

</xml_diff>